<commit_message>
reportes de temas dados
</commit_message>
<xml_diff>
--- a/ArchivosParaPruebas/Programa_Biologia_2020-2.xlsx
+++ b/ArchivosParaPruebas/Programa_Biologia_2020-2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\DayClass\ArchivosParaPruebas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{864CE3EB-AC16-4365-8BEB-63A3BB7DBE2C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF8C5540-4A3B-4CE3-8115-AA3BBEABA7D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A2D7B0D7-9458-4E5D-ACE9-981530461954}"/>
   </bookViews>
@@ -69,13 +69,13 @@
     <t>Células vegetales y células animales</t>
   </si>
   <si>
-    <t>La nutrición en el nivel celular: localización de los procesos de endocitosis, fotosíntesis y respiración celular.</t>
-  </si>
-  <si>
     <t>La diversidad biológica como consecuencia de la evolución.</t>
   </si>
   <si>
     <t>tema</t>
+  </si>
+  <si>
+    <t>La nutrición en el nivel celular: procesos de endocitosis, fotosíntesis y respiración celular.</t>
   </si>
 </sst>
 </file>
@@ -445,7 +445,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AD3FB17-EA56-4115-9C1C-E0E995912532}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -457,7 +459,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -569,7 +571,7 @@
         <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -585,7 +587,7 @@
         <v>6</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>